<commit_message>
log sheet updated ,added last update in project plane document
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/logsheet.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/logsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="390" windowWidth="10215" windowHeight="3720"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15495" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Reviewed sheet</t>
   </si>
@@ -72,6 +73,21 @@
   </si>
   <si>
     <t>The SRS is based on initial design and properly linked to CRS</t>
+  </si>
+  <si>
+    <t>project plan sheet</t>
+  </si>
+  <si>
+    <t>progress schedual needs to be updated</t>
+  </si>
+  <si>
+    <t>Ahmed adel</t>
+  </si>
+  <si>
+    <t>17/3/2016</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -139,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -292,6 +308,57 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -300,8 +367,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -314,6 +410,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -332,48 +437,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -677,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:I18"/>
+  <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -691,227 +791,264 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="20" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" thickTop="1">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="11" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:9">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="2:9">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:9">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="26"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="2:9">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="12" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="23"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="23"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="23"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="26"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="12" spans="2:9" ht="50.1" customHeight="1">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13" t="s">
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="35" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="17" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="36"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="24"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="36"/>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="24"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="36"/>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="24"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="36"/>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="24"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="36"/>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="25"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="37"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="30"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="31"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="I3:I6"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="H12:H18"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="I12:I18"/>
-    <mergeCell ref="G13:G18"/>
-    <mergeCell ref="D7:F11"/>
+  <mergeCells count="22">
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="B19:C21"/>
+    <mergeCell ref="D19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:H21"/>
     <mergeCell ref="B7:C11"/>
     <mergeCell ref="D12:F18"/>
     <mergeCell ref="B12:C18"/>
@@ -919,6 +1056,16 @@
     <mergeCell ref="D3:F6"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="B3:C6"/>
+    <mergeCell ref="H12:H18"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="I12:I18"/>
+    <mergeCell ref="G13:G18"/>
+    <mergeCell ref="D7:F11"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="I3:I6"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="H7:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>